<commit_message>
14 Nov (2nd commit)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdataexcel.xlsx
+++ b/src/test/resources/excel/testdataexcel.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="15075" windowHeight="3105" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15075" windowHeight="3105" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="8" r:id="rId1"/>
     <sheet name="AddCustomerTest" sheetId="9" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="10" r:id="rId3"/>
+    <sheet name="CreateContacts" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Rohan</t>
   </si>
@@ -94,6 +95,21 @@
   </si>
   <si>
     <t>firstname</t>
+  </si>
+  <si>
+    <t>companyname</t>
+  </si>
+  <si>
+    <t>CreateContacts</t>
+  </si>
+  <si>
+    <t>Sumitra</t>
+  </si>
+  <si>
+    <t>Dassault Systems 2</t>
+  </si>
+  <si>
+    <t>Dassault Systems 1</t>
   </si>
 </sst>
 </file>
@@ -425,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,7 +465,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -457,7 +473,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -465,6 +481,14 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -477,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,4 +641,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>